<commit_message>
reset zone + checkpoints
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbannister1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbannister1\workspace\AGA206\Roll-A-Ball\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -475,7 +475,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -519,7 +519,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$20" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2475,7 +2475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="55" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="55" workbookViewId="0">
       <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="D7" s="8">
         <f>COUNTIFS(J12:J15,TRUE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="D8" s="8">
         <f>COUNTIFS(J18:J38,TRUE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -2554,7 +2554,7 @@
       </c>
       <c r="D9" s="8">
         <f>K39</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2611,11 +2611,11 @@
       <c r="E13" s="7"/>
       <c r="F13" s="6" t="str">
         <f>IF(J13,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G13" s="17"/>
       <c r="J13" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2740,15 +2740,15 @@
       <c r="E20" s="7"/>
       <c r="F20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G20" s="17"/>
       <c r="J20" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
@@ -3186,7 +3186,7 @@
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3792,17 +3792,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c2062536-d537-4933-9a68-111b11088bac" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A5A66FD54D20CA4E9AC02DD318E94D49" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="53bde79962055b8cecc8a50be1004eac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de" xmlns:ns3="c2062536-d537-4933-9a68-111b11088bac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d9b45dcf71f2936b8953ced3331ea195" ns2:_="" ns3:_="">
     <xsd:import namespace="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de"/>
@@ -4045,6 +4034,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c2062536-d537-4933-9a68-111b11088bac" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14E3574E-6B93-421F-8C9B-EF2BAE2A1531}">
   <ds:schemaRefs>
@@ -4054,17 +4054,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F4C952-2792-4F13-AAE1-711BCAAD3EBE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c2062536-d537-4933-9a68-111b11088bac"/>
-    <ds:schemaRef ds:uri="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7E3157D-E74E-4DE5-B0FD-8DBD0694FA2F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4081,4 +4070,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F4C952-2792-4F13-AAE1-711BCAAD3EBE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c2062536-d537-4933-9a68-111b11088bac"/>
+    <ds:schemaRef ds:uri="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
more level stuff and particles
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -503,7 +503,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2475,7 +2475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="55" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="55" workbookViewId="0">
       <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="D7" s="8">
         <f>COUNTIFS(J12:J15,TRUE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
@@ -2631,11 +2631,11 @@
       <c r="E14" s="7"/>
       <c r="F14" s="6" t="str">
         <f>IF(J14,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G14" s="17"/>
       <c r="J14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3783,15 +3783,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A5A66FD54D20CA4E9AC02DD318E94D49" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="53bde79962055b8cecc8a50be1004eac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de" xmlns:ns3="c2062536-d537-4933-9a68-111b11088bac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d9b45dcf71f2936b8953ced3331ea195" ns2:_="" ns3:_="">
     <xsd:import namespace="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de"/>
@@ -4034,6 +4025,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4046,14 +4046,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14E3574E-6B93-421F-8C9B-EF2BAE2A1531}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7E3157D-E74E-4DE5-B0FD-8DBD0694FA2F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4072,6 +4064,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14E3574E-6B93-421F-8C9B-EF2BAE2A1531}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F4C952-2792-4F13-AAE1-711BCAAD3EBE}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
main menu, fixed rotation points and particles
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -431,7 +431,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="D7" s="8">
         <f>COUNTIFS(J12:J15,TRUE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
@@ -2591,11 +2591,11 @@
       <c r="E12" s="7"/>
       <c r="F12" s="6" t="str">
         <f>IF(J12,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G12" s="17"/>
       <c r="J12" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3783,6 +3783,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A5A66FD54D20CA4E9AC02DD318E94D49" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="53bde79962055b8cecc8a50be1004eac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de" xmlns:ns3="c2062536-d537-4933-9a68-111b11088bac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d9b45dcf71f2936b8953ced3331ea195" ns2:_="" ns3:_="">
     <xsd:import namespace="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de"/>
@@ -4025,15 +4034,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4046,6 +4046,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14E3574E-6B93-421F-8C9B-EF2BAE2A1531}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7E3157D-E74E-4DE5-B0FD-8DBD0694FA2F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4064,14 +4072,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14E3574E-6B93-421F-8C9B-EF2BAE2A1531}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F4C952-2792-4F13-AAE1-711BCAAD3EBE}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
new level and pause menu
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -435,11 +435,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$23" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$24" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$24" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
@@ -507,7 +507,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$15" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2475,8 +2475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="D7" s="8">
         <f>COUNTIFS(J12:J15,TRUE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="D8" s="8">
         <f>COUNTIFS(J18:J38,TRUE)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -2554,7 +2554,7 @@
       </c>
       <c r="D9" s="8">
         <f>K39</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2651,11 +2651,11 @@
       <c r="E15" s="7"/>
       <c r="F15" s="6" t="str">
         <f>IF(J15,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G15" s="17"/>
       <c r="J15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2812,15 +2812,15 @@
       <c r="E23" s="7"/>
       <c r="F23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G23" s="17"/>
       <c r="J23" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
@@ -2836,15 +2836,15 @@
       <c r="E24" s="7"/>
       <c r="F24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G24" s="17"/>
       <c r="J24" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
@@ -3186,7 +3186,7 @@
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3783,15 +3783,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A5A66FD54D20CA4E9AC02DD318E94D49" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="53bde79962055b8cecc8a50be1004eac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de" xmlns:ns3="c2062536-d537-4933-9a68-111b11088bac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d9b45dcf71f2936b8953ced3331ea195" ns2:_="" ns3:_="">
     <xsd:import namespace="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de"/>
@@ -4034,6 +4025,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4046,14 +4046,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14E3574E-6B93-421F-8C9B-EF2BAE2A1531}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7E3157D-E74E-4DE5-B0FD-8DBD0694FA2F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4072,6 +4064,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14E3574E-6B93-421F-8C9B-EF2BAE2A1531}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F4C952-2792-4F13-AAE1-711BCAAD3EBE}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
started second level and fixed mode bug
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbannister1\workspace\AGA206\Roll-A-Ball\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbannister1\Documents\GitHub\Roll-A-Ball\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>AGA206 Assessment 2 Checklist</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>Come up with your own</t>
+  </si>
+  <si>
+    <t>Added in a no checkpoint mode</t>
+  </si>
+  <si>
+    <t>Added a death counter</t>
+  </si>
+  <si>
+    <t>Just to add the points of the death counter being added</t>
   </si>
 </sst>
 </file>
@@ -479,7 +488,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$33" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$33" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
@@ -487,19 +496,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$35" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$35" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$35" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$35" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$35" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$35" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$35" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$35" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2475,8 +2484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2545,7 +2554,7 @@
       </c>
       <c r="D8" s="8">
         <f>COUNTIFS(J18:J38,TRUE)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -2554,7 +2563,7 @@
       </c>
       <c r="D9" s="8">
         <f>K39</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3052,15 +3061,17 @@
       <c r="E33" s="7"/>
       <c r="F33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G33" s="17"/>
+        <v>Done</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="J33" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
@@ -3100,15 +3111,17 @@
       <c r="E35" s="7"/>
       <c r="F35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G35" s="17"/>
+        <v>Done</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>35</v>
+      </c>
       <c r="J35" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
@@ -3150,7 +3163,9 @@
         <f t="shared" si="2"/>
         <v>To Be Done</v>
       </c>
-      <c r="G37" s="17"/>
+      <c r="G37" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="J37" s="5" t="b">
         <v>0</v>
       </c>
@@ -3186,7 +3201,7 @@
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -3783,6 +3798,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A5A66FD54D20CA4E9AC02DD318E94D49" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="53bde79962055b8cecc8a50be1004eac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de" xmlns:ns3="c2062536-d537-4933-9a68-111b11088bac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d9b45dcf71f2936b8953ced3331ea195" ns2:_="" ns3:_="">
     <xsd:import namespace="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de"/>
@@ -4025,15 +4049,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4046,6 +4061,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14E3574E-6B93-421F-8C9B-EF2BAE2A1531}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7E3157D-E74E-4DE5-B0FD-8DBD0694FA2F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4064,14 +4087,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14E3574E-6B93-421F-8C9B-EF2BAE2A1531}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F4C952-2792-4F13-AAE1-711BCAAD3EBE}">
   <ds:schemaRefs>

</xml_diff>